<commit_message>
Changed trade_id logic for exit
</commit_message>
<xml_diff>
--- a/UserProfile/excel/brijesh.xlsx
+++ b/UserProfile/excel/brijesh.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,16 +15,16 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DTD" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -31,22 +32,7 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
+    <font/>
     <font>
       <b val="1"/>
     </font>
@@ -59,7 +45,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -67,43 +53,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin"/>
       <right style="thin"/>
@@ -112,37 +62,36 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="number_style" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="number_style" xfId="1" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -505,73 +454,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="A1:XFD1048576"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n"/>
-      <c r="B1" s="1" t="n"/>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n"/>
-      <c r="B2" s="2" t="n"/>
-      <c r="C2" s="3" t="n"/>
-      <c r="D2" s="3" t="n"/>
-      <c r="E2" s="2" t="n"/>
-      <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="n"/>
-      <c r="H2" s="2" t="n"/>
-      <c r="I2" s="2" t="n"/>
-      <c r="J2" s="2" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n"/>
-      <c r="B3" s="2" t="n"/>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="2" t="n"/>
-      <c r="E3" s="2" t="n"/>
-      <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="n"/>
-      <c r="I3" s="2" t="n"/>
-      <c r="J3" s="2" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n"/>
-      <c r="B4" s="2" t="n"/>
-      <c r="C4" s="3" t="n"/>
-      <c r="D4" s="3" t="n"/>
-      <c r="E4" s="2" t="n"/>
-      <c r="F4" s="2" t="n"/>
-      <c r="G4" s="2" t="n"/>
-      <c r="H4" s="2" t="n"/>
-      <c r="I4" s="2" t="n"/>
-      <c r="J4" s="2" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="2" t="n"/>
-      <c r="E5" s="2" t="n"/>
-      <c r="F5" s="2" t="n"/>
-      <c r="G5" s="2" t="n"/>
-      <c r="H5" s="2" t="n"/>
-      <c r="I5" s="2" t="n"/>
-      <c r="J5" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -584,598 +476,838 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="8.77734375" customWidth="1" style="2" min="1" max="3"/>
-    <col width="17.6640625" bestFit="1" customWidth="1" style="2" min="4" max="5"/>
-    <col width="8.77734375" customWidth="1" style="2" min="6" max="6"/>
-    <col width="8.77734375" customWidth="1" style="2" min="7" max="16384"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>trade_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>trading_symbol</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>signal</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>entry_time</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>exit_time</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>entry_price</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>exit_price</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>hedge_entry_price</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>hedge_exit_price</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>trade_points</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>qty</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>pnl</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>tax</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>net_pnl</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>MP157</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>FINNIFTY31OCT23P19150</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="6" t="n">
         <v>45229.43819444445</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="6" t="n">
         <v>45229.44861111111</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="5" t="n">
         <v>73</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="5" t="n">
         <v>72.51000000000001</v>
       </c>
-      <c r="H2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6" t="n">
+      <c r="H2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="n">
         <v>-0.49</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="1" t="n">
         <v>480</v>
       </c>
-      <c r="L2" s="6" t="n">
+      <c r="L2" s="5" t="n">
         <v>-235.2</v>
       </c>
-      <c r="M2" s="6" t="n">
+      <c r="M2" s="5" t="n">
         <v>78.77</v>
       </c>
-      <c r="N2" s="6" t="n">
+      <c r="N2" s="5" t="n">
         <v>-313.97</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>MP158</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>NIFTY02NOV23P19100</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="6" t="n">
         <v>45229.45</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="6" t="n">
         <v>45229.47986111111</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="5" t="n">
         <v>93.75</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="5" t="n">
         <v>76.40000000000001</v>
       </c>
-      <c r="H3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6" t="n">
+      <c r="H3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5" t="n">
         <v>-17.35</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="L3" s="6" t="n">
+      <c r="L3" s="5" t="n">
         <v>-7807.5</v>
       </c>
-      <c r="M3" s="6" t="n">
+      <c r="M3" s="5" t="n">
         <v>78.23999999999999</v>
       </c>
-      <c r="N3" s="6" t="n">
+      <c r="N3" s="5" t="n">
         <v>-7885.74</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>MP159</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>BANKNIFTY01NOV23P43000</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="6" t="n">
         <v>45230.43263888889</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="6" t="n">
         <v>45230.5125</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="5" t="n">
         <v>186.5</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="5" t="n">
         <v>186</v>
       </c>
-      <c r="H4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="n">
+      <c r="H4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5" t="n">
         <v>-0.5</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="L4" s="6" t="n">
+      <c r="L4" s="5" t="n">
         <v>-60</v>
       </c>
-      <c r="M4" s="6" t="n">
+      <c r="M4" s="5" t="n">
         <v>63.21</v>
       </c>
-      <c r="N4" s="6" t="n">
+      <c r="N4" s="5" t="n">
         <v>-123.21</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>MP160</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>NIFTY02NOV23P19100</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="6" t="n">
         <v>45230.43263888889</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="6" t="n">
         <v>45230.54861111111</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="5" t="n">
         <v>87.59999999999999</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="5" t="n">
         <v>67.2</v>
       </c>
-      <c r="H5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6" t="n">
+      <c r="H5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5" t="n">
         <v>-20.4</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="L5" s="6" t="n">
+      <c r="L5" s="5" t="n">
         <v>-8160</v>
       </c>
-      <c r="M5" s="6" t="n">
+      <c r="M5" s="5" t="n">
         <v>68.90000000000001</v>
       </c>
-      <c r="N5" s="6" t="n">
+      <c r="N5" s="5" t="n">
         <v>-8228.9</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>MP161</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>FINNIFTY07NOV23P19100</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C6" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="6" t="n">
         <v>45231.46875</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="6" t="n">
         <v>45231.51875</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="5" t="n">
         <v>110</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="5" t="n">
         <v>83.59999999999999</v>
       </c>
-      <c r="H6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6" t="n">
+      <c r="H6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5" t="n">
         <v>-26.4</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="L6" s="6" t="n">
+      <c r="L6" s="5" t="n">
         <v>-10560</v>
       </c>
-      <c r="M6" s="6" t="n">
+      <c r="M6" s="5" t="n">
         <v>77.06999999999999</v>
       </c>
-      <c r="N6" s="6" t="n">
+      <c r="N6" s="5" t="n">
         <v>-10637.07</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>MP162</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>BANKNIFTY01NOV23P42600</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="6" t="n">
         <v>45231.46944444445</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="6" t="n">
         <v>45231.62569444445</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="5" t="n">
         <v>52.7</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="G7" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6" t="n">
+      <c r="H7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5" t="n">
         <v>-50.7</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="K7" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="L7" s="6" t="n">
+      <c r="L7" s="5" t="n">
         <v>-6084</v>
       </c>
-      <c r="M7" s="6" t="n">
+      <c r="M7" s="5" t="n">
         <v>35.7</v>
       </c>
-      <c r="N7" s="6" t="n">
+      <c r="N7" s="5" t="n">
         <v>-6119.7</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>MP163</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>NIFTY02NOV23P19100</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="C8" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="6" t="n">
         <v>45232.48402777778</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="6" t="n">
         <v>45232.61944444444</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="5" t="n">
         <v>24.05</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6" t="n">
+      <c r="H8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5" t="n">
         <v>-22.05</v>
       </c>
-      <c r="K8" s="2" t="n">
+      <c r="K8" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="L8" s="6" t="n">
+      <c r="L8" s="5" t="n">
         <v>-6615</v>
       </c>
-      <c r="M8" s="6" t="n">
+      <c r="M8" s="5" t="n">
         <v>36.15</v>
       </c>
-      <c r="N8" s="6" t="n">
+      <c r="N8" s="5" t="n">
         <v>-6651.15</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>MP164</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B9" s="1" t="inlineStr">
         <is>
           <t>BANKNIFTY08NOV23P43000</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="C9" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="6" t="n">
         <v>45232.4875</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="6" t="n">
         <v>45232.59444444445</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="5" t="n">
         <v>291.45</v>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="5" t="n">
         <v>246</v>
       </c>
-      <c r="H9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6" t="n">
+      <c r="H9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5" t="n">
         <v>-45.45</v>
       </c>
-      <c r="K9" s="2" t="n">
+      <c r="K9" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="L9" s="6" t="n">
+      <c r="L9" s="5" t="n">
         <v>-4090.5</v>
       </c>
-      <c r="M9" s="6" t="n">
+      <c r="M9" s="5" t="n">
         <v>62.99</v>
       </c>
-      <c r="N9" s="6" t="n">
+      <c r="N9" s="5" t="n">
         <v>-4153.49</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>MP165</t>
         </is>
       </c>
-      <c r="B10" s="2" t="inlineStr">
+      <c r="B10" s="1" t="inlineStr">
         <is>
           <t>NIFTY09NOV23C19250</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
+      <c r="C10" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D10" s="5" t="inlineStr">
-        <is>
-          <t>2023-11-03 10:58:00</t>
-        </is>
-      </c>
-      <c r="E10" s="5" t="inlineStr">
-        <is>
-          <t>2023-11-03 11:52:00</t>
-        </is>
-      </c>
-      <c r="F10" s="6" t="n">
+      <c r="D10" s="6" t="n">
+        <v>45233.45694444444</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>45233.49444444444</v>
+      </c>
+      <c r="F10" s="5" t="n">
         <v>110.26</v>
       </c>
-      <c r="G10" s="6" t="n">
+      <c r="G10" s="5" t="n">
         <v>96.7</v>
       </c>
-      <c r="H10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6" t="n">
+      <c r="H10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5" t="n">
         <v>-13.56</v>
       </c>
-      <c r="K10" s="2" t="n">
+      <c r="K10" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="L10" s="6" t="n">
+      <c r="L10" s="5" t="n">
         <v>-6780</v>
       </c>
-      <c r="M10" s="6" t="n">
+      <c r="M10" s="5" t="n">
         <v>95.65000000000001</v>
       </c>
-      <c r="N10" s="6" t="n">
+      <c r="N10" s="5" t="n">
         <v>-6875.65</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>MP166</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="B11" s="1" t="inlineStr">
         <is>
           <t>BANKNIFTY08NOV23C43400</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
+      <c r="C11" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>2023-11-03 10:58:00</t>
-        </is>
-      </c>
-      <c r="E11" s="5" t="inlineStr">
-        <is>
-          <t>2023-11-03 11:18:00</t>
-        </is>
-      </c>
-      <c r="F11" s="6" t="n">
+      <c r="D11" s="6" t="n">
+        <v>45233.45694444444</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>45233.47083333333</v>
+      </c>
+      <c r="F11" s="5" t="n">
         <v>243.74</v>
       </c>
-      <c r="G11" s="6" t="n">
+      <c r="G11" s="5" t="n">
         <v>202.34</v>
       </c>
-      <c r="H11" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6" t="n">
+      <c r="H11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5" t="n">
         <v>-41.4</v>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="K11" s="1" t="n">
         <v>195</v>
       </c>
-      <c r="L11" s="6" t="n">
+      <c r="L11" s="5" t="n">
         <v>-8073</v>
       </c>
-      <c r="M11" s="6" t="n">
+      <c r="M11" s="5" t="n">
         <v>84.56999999999999</v>
       </c>
-      <c r="N11" s="6" t="n">
+      <c r="N11" s="5" t="n">
         <v>-8157.57</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>MP41</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY09NOV23P19250</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>45235.59791666667</v>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v>45235.59791666667</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="L12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="N12" s="5" t="n">
+        <v>-35.4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>MP41</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY09NOV23P19250</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D13" s="6" t="n">
+        <v>45235.59791666667</v>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>45235.59791666667</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="N13" s="5" t="n">
+        <v>-35.4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>MP41</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY09NOV23P19250</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v>45235.59791666667</v>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>45235.59791666667</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="L14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="N14" s="5" t="n">
+        <v>-35.4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>MP41</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY09NOV23P19250</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>45235.59791666667</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>45235.59791666667</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="N15" s="5" t="n">
+        <v>-35.4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>MP41</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY09NOV23P19250</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>2023-11-05 14:21:00</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>2023-11-05 14:21:00</t>
+        </is>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="N16" s="5" t="n">
+        <v>-35.4</v>
       </c>
     </row>
   </sheetData>
@@ -1189,344 +1321,588 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="8.77734375" customWidth="1" style="2" min="1" max="3"/>
-    <col width="17.6640625" bestFit="1" customWidth="1" style="2" min="4" max="5"/>
-    <col width="8.77734375" customWidth="1" style="2" min="6" max="6"/>
-    <col width="8.77734375" customWidth="1" style="2" min="7" max="16384"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>trade_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>trading_symbol Symbol</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>signal</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>entry_time</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>exit_time</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>entry_price</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>exit_price</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>hedge_entry_price</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>hedge_exit_price</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>trade_points</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>qty</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>pnl</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>tax</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>net_pnl</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>AP75</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NIFTY23N0218500PE</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="6" t="n">
         <v>45229.38958333333</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="6" t="n">
         <v>45229.62222222222</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="5" t="n">
         <v>207</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="5" t="n">
         <v>224.8</v>
       </c>
-      <c r="H2" s="6" t="n">
+      <c r="H2" s="5" t="n">
         <v>12.2</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="5" t="n">
         <v>9.85</v>
       </c>
-      <c r="J2" s="6" t="n">
+      <c r="J2" s="5" t="n">
         <v>-20.15</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L2" s="6" t="n">
+      <c r="L2" s="5" t="n">
         <v>-2015</v>
       </c>
-      <c r="M2" s="6" t="n">
+      <c r="M2" s="5" t="n">
         <v>173.07</v>
       </c>
-      <c r="N2" s="6" t="n">
+      <c r="N2" s="5" t="n">
         <v>-2188.07</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>AP76</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>NIFTY02NOV23P19200</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="6" t="n">
         <v>45230.39375</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="6" t="n">
         <v>45230.62222222222</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="5" t="n">
         <v>172.66</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="5" t="n">
         <v>149.9</v>
       </c>
-      <c r="H3" s="6" t="n">
+      <c r="H3" s="5" t="n">
         <v>9.050000000000001</v>
       </c>
-      <c r="I3" s="6" t="n">
+      <c r="I3" s="5" t="n">
         <v>6.1</v>
       </c>
-      <c r="J3" s="6" t="n">
+      <c r="J3" s="5" t="n">
         <v>19.81</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="L3" s="6" t="n">
+      <c r="L3" s="5" t="n">
         <v>2971.5</v>
       </c>
-      <c r="M3" s="6" t="n">
+      <c r="M3" s="5" t="n">
         <v>170.76</v>
       </c>
-      <c r="N3" s="6" t="n">
+      <c r="N3" s="5" t="n">
         <v>2800.74</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>AP77</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>NIFTY02NOV23P19100</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="6" t="n">
         <v>45231.40347222222</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="6" t="n">
         <v>45231.61458333334</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="5" t="n">
         <v>139.95</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="5" t="n">
         <v>140.5</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H4" s="5" t="n">
         <v>4.95</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="5" t="n">
         <v>2.7</v>
       </c>
-      <c r="J4" s="6" t="n">
+      <c r="J4" s="5" t="n">
         <v>-2.8</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="L4" s="6" t="n">
+      <c r="L4" s="5" t="n">
         <v>-420</v>
       </c>
-      <c r="M4" s="6" t="n">
+      <c r="M4" s="5" t="n">
         <v>168.47</v>
       </c>
-      <c r="N4" s="6" t="n">
+      <c r="N4" s="5" t="n">
         <v>-588.47</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>AP78</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>NIFTY02NOV23P19100</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="6" t="n">
         <v>45232.38958333333</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="6" t="n">
         <v>45232.62222222222</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="5" t="n">
         <v>82</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="5" t="n">
         <v>29.1</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="5" t="n">
         <v>1.1</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="J5" s="5" t="n">
         <v>51.9</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="L5" s="6" t="n">
+      <c r="L5" s="5" t="n">
         <v>7785</v>
       </c>
-      <c r="M5" s="6" t="n">
+      <c r="M5" s="5" t="n">
         <v>147.06</v>
       </c>
-      <c r="N5" s="6" t="n">
+      <c r="N5" s="5" t="n">
         <v>7637.94</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>AP79</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>NIFTY23N0919200CE</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C6" s="1" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
-        <is>
-          <t>2023-11-03 09:21:00</t>
-        </is>
-      </c>
-      <c r="E6" s="5" t="inlineStr">
-        <is>
-          <t>2023-11-03 14:56:00</t>
-        </is>
-      </c>
-      <c r="F6" s="6" t="n">
+      <c r="D6" s="6" t="n">
+        <v>45233.38958333333</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>45233.62222222222</v>
+      </c>
+      <c r="F6" s="5" t="n">
         <v>213.37</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="5" t="n">
         <v>192.2</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="5" t="n">
         <v>9.5</v>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I6" s="5" t="n">
         <v>8.25</v>
       </c>
-      <c r="J6" s="6" t="n">
+      <c r="J6" s="5" t="n">
         <v>19.92</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="L6" s="6" t="n">
+      <c r="L6" s="5" t="n">
         <v>2988</v>
       </c>
-      <c r="M6" s="6" t="n">
+      <c r="M6" s="5" t="n">
         <v>179.07</v>
       </c>
-      <c r="N6" s="6" t="n">
+      <c r="N6" s="5" t="n">
         <v>2808.93</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>AP36</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY09NOV23P19200</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>45235.59444444445</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>45235.59583333333</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>141.6</v>
+      </c>
+      <c r="N7" s="5" t="n">
+        <v>-141.6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>AP36</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY09NOV23P19200</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>45235.59444444445</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>45235.59583333333</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5" t="n">
+        <v>141.6</v>
+      </c>
+      <c r="N8" s="5" t="n">
+        <v>-141.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>AP36</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY09NOV23P19200</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>45235.59444444445</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>45235.59583333333</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5" t="n">
+        <v>141.6</v>
+      </c>
+      <c r="N9" s="5" t="n">
+        <v>-141.6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>AP36</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY09NOV23P19200</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>45235.59444444445</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>45235.59583333333</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5" t="n">
+        <v>141.6</v>
+      </c>
+      <c r="N10" s="5" t="n">
+        <v>-141.6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>AP36</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY09NOV23P19200</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>2023-11-05 14:16:00</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="inlineStr">
+        <is>
+          <t>2023-11-05 14:18:00</t>
+        </is>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5" t="n">
+        <v>141.6</v>
+      </c>
+      <c r="N11" s="5" t="n">
+        <v>-141.6</v>
       </c>
     </row>
   </sheetData>
@@ -1540,299 +1916,321 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="8.77734375" customWidth="1" style="2" min="1" max="3"/>
-    <col width="17.6640625" bestFit="1" customWidth="1" style="2" min="4" max="5"/>
-    <col width="8.77734375" customWidth="1" style="2" min="6" max="6"/>
-    <col width="8.77734375" customWidth="1" style="2" min="7" max="11"/>
-    <col width="9.21875" bestFit="1" customWidth="1" style="2" min="12" max="12"/>
-    <col width="8.77734375" customWidth="1" style="2" min="13" max="13"/>
-    <col width="9.21875" bestFit="1" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.77734375" customWidth="1" style="2" min="15" max="16384"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>trade_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>trading_symbol</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>signal</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>entry_time</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>exit_time</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>entry_price</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>exit_price</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>hedge_entry_price</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>hedge_exit_price</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>trade_points</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>qty</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>pnl</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>tax</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>net_pnl</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>OO28</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NIFTY30NOV23F</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="6" t="n">
         <v>45229.63541666666</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="6" t="n">
         <v>45230.3875</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="5" t="n">
         <v>19210.8</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="5" t="n">
         <v>19236.65</v>
       </c>
-      <c r="H2" s="6" t="n">
+      <c r="H2" s="5" t="n">
         <v>30.4</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="5" t="n">
         <v>38.6</v>
       </c>
-      <c r="J2" s="6" t="n">
+      <c r="J2" s="5" t="n">
         <v>-17.65</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L2" s="6" t="n">
+      <c r="L2" s="5" t="n">
         <v>-1765</v>
       </c>
-      <c r="M2" s="6" t="n">
+      <c r="M2" s="5" t="n">
         <v>572.25</v>
       </c>
-      <c r="N2" s="6" t="n">
+      <c r="N2" s="5" t="n">
         <v>-2337.25</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>OO29</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>NIFTY30NOV23F</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="6" t="n">
         <v>45230.63541666666</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="6" t="n">
         <v>45231.3875</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="5" t="n">
         <v>19199.06</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="5" t="n">
         <v>19151.3</v>
       </c>
-      <c r="H3" s="6" t="n">
+      <c r="H3" s="5" t="n">
         <v>26.6</v>
       </c>
-      <c r="I3" s="6" t="n">
+      <c r="I3" s="5" t="n">
         <v>27.77</v>
       </c>
-      <c r="J3" s="6" t="n">
+      <c r="J3" s="5" t="n">
         <v>-46.59</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L3" s="6" t="n">
+      <c r="L3" s="5" t="n">
         <v>-4659</v>
       </c>
-      <c r="M3" s="6" t="n">
+      <c r="M3" s="5" t="n">
         <v>568.76</v>
       </c>
-      <c r="N3" s="6" t="n">
+      <c r="N3" s="5" t="n">
         <v>-5227.76</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>OO30</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>NIFTY30NOV23F</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="6" t="n">
         <v>44937.63541666666</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="6" t="n">
         <v>45232.3875</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="5" t="n">
         <v>19056.88</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="5" t="n">
         <v>19221.27</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H4" s="5" t="n">
         <v>8.300000000000001</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="J4" s="6" t="n">
+      <c r="J4" s="5" t="n">
         <v>-141.7</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L4" s="6" t="n">
+      <c r="L4" s="5" t="n">
         <v>-14169.5</v>
       </c>
-      <c r="M4" s="6" t="n">
+      <c r="M4" s="5" t="n">
         <v>572.89</v>
       </c>
-      <c r="N4" s="6" t="n">
+      <c r="N4" s="5" t="n">
         <v>-14742.39</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>OO31</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>NIFTY30NOV23F</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>2023-11-03 15:15:00</t>
-        </is>
-      </c>
-      <c r="E5" s="5" t="inlineStr">
-        <is>
-          <t>2023-11-03 09:18:00</t>
-        </is>
-      </c>
-      <c r="F5" s="6" t="n">
+      <c r="D5" s="6" t="n">
+        <v>45233.63541666666</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>45233.3875</v>
+      </c>
+      <c r="F5" s="5" t="n">
         <v>19228.45</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="5" t="n">
         <v>19347.5</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="5" t="n">
         <v>35.1</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="5" t="n">
         <v>14.15</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="J5" s="5" t="n">
         <v>98.09999999999999</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L5" s="6" t="n">
+      <c r="L5" s="5" t="n">
         <v>9810</v>
       </c>
-      <c r="M5" s="6" t="n">
+      <c r="M5" s="5" t="n">
         <v>569.8099999999999</v>
       </c>
-      <c r="N5" s="6" t="n">
+      <c r="N5" s="5" t="n">
         <v>9240.190000000001</v>
       </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>OO28</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>NIFTY30NOV23F</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>45235.60486111111</v>
+      </c>
+      <c r="E6" s="1" t="inlineStr"/>
+      <c r="F6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="inlineStr"/>
+      <c r="H6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="inlineStr"/>
+      <c r="J6" s="5" t="inlineStr"/>
+      <c r="K6" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="L6" s="5" t="inlineStr"/>
+      <c r="M6" s="5" t="inlineStr"/>
+      <c r="N6" s="5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1851,277 +2249,277 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>trade_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>trading_symbol</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>signal</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>entry_time</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>exit_time</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>entry_price</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>exit_price</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>hedge_entry_price</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>hedge_exit_price</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>trade_points</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>qty</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>pnl</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>tax</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>net_pnl</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Error1</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NIFTY23N0218500PE</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="6" t="n">
         <v>45229.38958333333</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="6" t="n">
         <v>45229.38958333333</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="F2" s="5" t="n">
         <v>8.199999999999999</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="5" t="n">
         <v>8.75</v>
       </c>
-      <c r="H2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4" t="n">
+      <c r="H2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="n">
         <v>-0.55</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="L2" s="5" t="n">
         <v>-55</v>
       </c>
-      <c r="M2" s="4" t="n">
+      <c r="M2" s="5" t="n">
         <v>43.62</v>
       </c>
-      <c r="N2" s="4" t="n">
+      <c r="N2" s="5" t="n">
         <v>-98.62</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Error2</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>NIFTY23N0219500CE</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="6" t="n">
         <v>45229.38958333333</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="6" t="n">
         <v>45229.38958333333</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="5" t="n">
         <v>4.25</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="5" t="n">
         <v>3.45</v>
       </c>
-      <c r="H3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4" t="n">
+      <c r="H3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5" t="n">
         <v>0.8</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L3" s="4" t="n">
+      <c r="L3" s="5" t="n">
         <v>80</v>
       </c>
-      <c r="M3" s="4" t="n">
+      <c r="M3" s="5" t="n">
         <v>42.69</v>
       </c>
-      <c r="N3" s="4" t="n">
+      <c r="N3" s="5" t="n">
         <v>37.31</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>Error3</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>BANKNIFTY01NOV23P42600</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="6" t="n">
         <v>45231.46597222222</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="6" t="n">
         <v>45231.46597222222</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="5" t="n">
         <v>64.45999999999999</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="5" t="n">
         <v>60.05</v>
       </c>
-      <c r="H4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4" t="n">
+      <c r="H4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5" t="n">
         <v>-4.41</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="L4" s="4" t="n">
+      <c r="L4" s="5" t="n">
         <v>-529.2</v>
       </c>
-      <c r="M4" s="4" t="n">
+      <c r="M4" s="5" t="n">
         <v>35.44</v>
       </c>
-      <c r="N4" s="4" t="n">
+      <c r="N4" s="5" t="n">
         <v>-564.64</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>Error4</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>FINNIFTY07NOV23P19100</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="6" t="n">
         <v>45231.46597222222</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="6" t="n">
         <v>45231.46666666667</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="5" t="n">
         <v>112.07</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="5" t="n">
         <v>106.85</v>
       </c>
-      <c r="H5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4" t="n">
+      <c r="H5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5" t="n">
         <v>-5.22</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="L5" s="4" t="n">
+      <c r="L5" s="5" t="n">
         <v>-2088</v>
       </c>
-      <c r="M5" s="4" t="n">
+      <c r="M5" s="5" t="n">
         <v>43.72</v>
       </c>
-      <c r="N5" s="4" t="n">
+      <c r="N5" s="5" t="n">
         <v>-2131.72</v>
       </c>
     </row>
@@ -2136,7 +2534,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2145,37 +2543,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Sl NO</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Day</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Trade ID</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>Details</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="F1" s="7" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="G1" s="7" t="inlineStr">
         <is>
           <t>Running Balance</t>
         </is>
@@ -3014,6 +3412,356 @@
       <c r="G25" t="inlineStr">
         <is>
           <t>₹ 5,29,430.24</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>05-Nov-23</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>MP41</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>MPWizard</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>-₹35.40</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>₹5,29,394.84</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>05-Nov-23</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>MP41</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>MPWizard</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-₹35.40</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>₹5,29,359.44</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>05-Nov-23</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>MP41</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>MPWizard</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-₹35.40</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>₹5,29,324.04</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>05-Nov-23</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>MP41</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>MPWizard</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-₹35.40</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>₹5,29,288.64</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>05-Nov-23</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>MP41</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>MPWizard</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>-₹35.40</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>₹5,29,253.24</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>05-Nov-23</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>AP36</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>AmiPy</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>-₹141.60</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>₹5,29,111.64</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>05-Nov-23</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>AP36</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>AmiPy</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>-₹141.60</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>₹5,28,970.04</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>05-Nov-23</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>AP36</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>AmiPy</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>-₹141.60</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>₹5,28,828.44</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>05-Nov-23</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>AP36</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>AmiPy</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>-₹141.60</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>₹5,28,686.84</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>05-Nov-23</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>AP36</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>AmiPy</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>-₹141.60</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>₹5,28,545.24</t>
         </is>
       </c>
     </row>

</xml_diff>